<commit_message>
Amendements de style divers et ajout de matériaux à la base de données
</commit_message>
<xml_diff>
--- a/docs/base_de_donnees_materiaux/bdd-materiaux.xlsx
+++ b/docs/base_de_donnees_materiaux/bdd-materiaux.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base de donnees materiaux/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clement/Workspace/cpoc-at-omc/docs/base_de_donnees_materiaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7614EB13-9A39-DD45-A5FB-2C24C04B288F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6949EFD-E128-8845-B3DA-235300932447}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="460" windowWidth="20700" windowHeight="14560" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20320" yWindow="460" windowWidth="20320" windowHeight="14340" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="263">
   <si>
     <t>Matériau</t>
   </si>
@@ -828,6 +828,9 @@
   </si>
   <si>
     <t>bien Anodisable, bel aspect. Bonne tenue à la corrosion, très bien soudable, mauvaise fragmebtabilité du copeau et mauvaise capacité d'emboutissage.  Mal usinable</t>
+  </si>
+  <si>
+    <t>de 10 à 13</t>
   </si>
 </sst>
 </file>
@@ -1843,24 +1846,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F9ECE-8D5C-814E-98CE-0956327B3220}">
   <dimension ref="B1:Z28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="17" width="10.83203125" style="1"/>
-    <col min="18" max="18" width="98.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="15" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="98.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
-    <col min="25" max="25" width="13.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="14.83203125" style="1" customWidth="1"/>
     <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1989,6 +1998,9 @@
       <c r="K3" s="1">
         <v>240</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="P3" s="1">
         <v>1300</v>
       </c>
@@ -2000,6 +2012,9 @@
       </c>
       <c r="U3" s="1">
         <v>4</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1</v>
       </c>
       <c r="Z3" s="1">
         <v>2</v>
@@ -2084,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="V5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z5" s="1">
         <v>2</v>
@@ -2125,7 +2140,7 @@
         <v>2</v>
       </c>
       <c r="V6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Z6" s="1">
         <v>3</v>
@@ -2169,7 +2184,7 @@
         <v>5</v>
       </c>
       <c r="V7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Z7" s="1">
         <v>3</v>
@@ -2267,6 +2282,9 @@
       <c r="K10" s="1">
         <v>217</v>
       </c>
+      <c r="L10" s="1">
+        <v>10</v>
+      </c>
       <c r="P10" s="1">
         <v>1300</v>
       </c>
@@ -2372,14 +2390,17 @@
       <c r="C13" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="I13" s="1">
+        <v>590</v>
+      </c>
       <c r="J13" s="1">
-        <v>980</v>
+        <v>975</v>
       </c>
       <c r="K13" s="1">
-        <v>235</v>
+        <v>280</v>
       </c>
       <c r="L13" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P13" s="1">
         <v>1820</v>
@@ -2416,6 +2437,9 @@
       <c r="J14" s="1">
         <v>1000</v>
       </c>
+      <c r="K14" s="1">
+        <v>217</v>
+      </c>
       <c r="L14" s="1">
         <v>11</v>
       </c>
@@ -2560,6 +2584,9 @@
       <c r="U17" s="1">
         <v>4</v>
       </c>
+      <c r="V17" s="1">
+        <v>3</v>
+      </c>
       <c r="W17" s="1">
         <v>4</v>
       </c>
@@ -2685,6 +2712,9 @@
       </c>
       <c r="U20" s="1">
         <v>3</v>
+      </c>
+      <c r="V20" s="1">
+        <v>1</v>
       </c>
       <c r="Z20" s="1">
         <v>1</v>
@@ -2877,8 +2907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084ADA29-3FC8-704E-AEA5-3C9B0E480466}">
   <dimension ref="B1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
@@ -3328,11 +3358,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50E0626-187A-8641-B3DB-E474EE2CB96A}">
   <dimension ref="B1:Z9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3493,6 +3523,9 @@
       <c r="X3" s="1">
         <v>3</v>
       </c>
+      <c r="Z3" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="2:26" ht="30">
       <c r="B4" s="1" t="s">
@@ -3650,6 +3683,9 @@
       </c>
       <c r="U7" s="1">
         <v>2</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:26" ht="30">

</xml_diff>